<commit_message>
Updated Excel Sheet + Added BubbleStateDiagram
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyounjun\Desktop\CU_Boulder\ECEN5823\assignments\ecen5823_workspace\ecen5823-assignment6-hyounjunchang\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF36A889-3049-4DE4-879E-2A5FE18051B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289E3C16-C039-4F57-81C7-644C22BB4449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -167,22 +167,13 @@
     <t>Start scanning for server again (for new potential connection)</t>
   </si>
   <si>
-    <t>Indication enabled for Temperature Measurement (uuid = 0x2A1C)</t>
-  </si>
-  <si>
     <t>Look for Temperature Measurement Characteristic (uuid = 0x2A1C)</t>
   </si>
   <si>
-    <t>Discovered Health Thermometer Service(uuid = 0x1809)</t>
-  </si>
-  <si>
     <t>sl_bt_gatt_set_characteristic_notification()</t>
   </si>
   <si>
     <t>Set indication for Temp. Measurement (uuid = 0x2A1C)</t>
-  </si>
-  <si>
-    <t>Discovered Temperature Measurement Characteristic (uuid = 0x2A1C)</t>
   </si>
   <si>
     <r>
@@ -255,14 +246,23 @@
     </r>
   </si>
   <si>
-    <t>Do not call if it's for indication update</t>
+    <t>Discovered Temperature Measurement Characteristic (uuid = 0x2A1C), store data for state update later</t>
+  </si>
+  <si>
+    <t>Indication enabled for Temperature Measurement (uuid = 0x2A1C), store data for state update later</t>
+  </si>
+  <si>
+    <t>Discovered Health Thermometer Service(uuid = 0x1809), store data for state update later</t>
+  </si>
+  <si>
+    <t>Only for temperature indication</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -296,11 +296,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="14"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color indexed="14"/>
       <name val="Calibri"/>
     </font>
@@ -468,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -514,10 +509,7 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -525,19 +517,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1713,10 +1705,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="87" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1733,13 +1725,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1760,7 +1752,7 @@
       <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>36</v>
       </c>
       <c r="F3" s="5"/>
@@ -1800,7 +1792,7 @@
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="12" t="s">
@@ -1812,7 +1804,7 @@
       <c r="B7" s="4"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="31" t="s">
         <v>32</v>
       </c>
       <c r="F7" s="12" t="s">
@@ -1824,7 +1816,7 @@
       <c r="B8" s="4"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="32"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="15" t="s">
         <v>14</v>
       </c>
@@ -1834,7 +1826,7 @@
       <c r="B9" s="4"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="32"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1884,16 +1876,16 @@
       <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="22" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1935,11 +1927,11 @@
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
-      <c r="E18" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>49</v>
+      <c r="E18" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1966,128 +1958,106 @@
         <v>23</v>
       </c>
       <c r="C21" s="16"/>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="16"/>
-    </row>
-    <row r="23" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-    </row>
-    <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E24" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="17" t="s">
-        <v>27</v>
-      </c>
+      <c r="B25" s="4"/>
       <c r="C25" s="16"/>
-      <c r="D25" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>28</v>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="F25" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+      <c r="B26" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="27" t="s">
-        <v>38</v>
+      <c r="D26" s="26"/>
+      <c r="E26" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C27" s="16"/>
-      <c r="D27" s="27" t="s">
-        <v>34</v>
-      </c>
+      <c r="D27" s="26"/>
       <c r="E27" s="18" t="s">
         <v>30</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="B28" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="25" t="s">
         <v>44</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="F30" s="27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified i2c/scheduler code to separate server code from client code added diagram to command table for A7
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyounjun\Desktop\CU_Boulder\ECEN5823\assignments\ecen5823_workspace\ecen5823-assignment6-hyounjunchang\questions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyounjun\Desktop\CU_Boulder\ECEN5823\assignments\ecen5823_workspace\ecen5823-assignment7-hyounjunchang\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289E3C16-C039-4F57-81C7-644C22BB4449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE7E1B4-3CD6-4955-BF75-EB1C2FA7A4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2685" yWindow="2685" windowWidth="24885" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -627,6 +627,61 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>821121</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>32844</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1520935</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>115353</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{406AF408-2E0B-60C7-7199-ED406DA2ADDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="821121" y="10959223"/>
+          <a:ext cx="7772400" cy="5162509"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -1707,8 +1762,8 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="87" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="87" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2032,7 +2087,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="17" t="s">
         <v>29</v>
@@ -2046,7 +2101,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="17" t="s">
         <v>31</v>
@@ -2070,5 +2125,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified event to sl_bt_evt_scanner_legacy_advertisement_report_id Added log statements(to be removed later) added LETIMER for client for logging
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyounjun\Desktop\CU_Boulder\ECEN5823\assignments\ecen5823_workspace\ecen5823-assignment7-hyounjunchang\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE7E1B4-3CD6-4955-BF75-EB1C2FA7A4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB0EFB1-FAED-4C70-9EFB-34C096E3B4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2685" yWindow="2685" windowWidth="24885" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="6105" windowWidth="24885" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Events only for Masters/Clients</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_scanner_scan_report_id</t>
   </si>
   <si>
     <t>sl_bt_evt_gatt_procedure_completed_id</t>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>Only for temperature indication</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_scanner_legacy_advertisement_report_id</t>
   </si>
 </sst>
 </file>
@@ -1762,8 +1762,8 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="87" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="87" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1808,7 +1808,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="5"/>
     </row>
@@ -1860,7 +1860,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>13</v>
@@ -1883,7 +1883,7 @@
       <c r="D9" s="13"/>
       <c r="E9" s="31"/>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1903,7 +1903,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>17</v>
@@ -1935,13 +1935,13 @@
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
       <c r="D14" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1958,13 +1958,13 @@
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1983,10 +1983,10 @@
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2010,31 +2010,31 @@
     <row r="21" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="17" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2043,10 +2043,10 @@
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
       <c r="E23" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2055,10 +2055,10 @@
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2067,52 +2067,52 @@
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="16" t="s">
         <v>42</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="26"/>
       <c r="E26" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="26"/>
       <c r="E27" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
       <c r="E28" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated command table excel sheet for A7 connection_closed_id always resets state to CLIENT_SCANNING
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyounjun\Desktop\CU_Boulder\ECEN5823\assignments\ecen5823_workspace\ecen5823-assignment7-hyounjunchang\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB0EFB1-FAED-4C70-9EFB-34C096E3B4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7109FB-EC01-4C65-A003-CC5967669A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="6105" windowWidth="24885" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -103,15 +103,9 @@
     <t>sl_bt_evt_gatt_service_id</t>
   </si>
   <si>
-    <t>A GATT service in the remote GATT database was discovered</t>
-  </si>
-  <si>
     <t>sl_bt_evt_gatt_characteristic_id</t>
   </si>
   <si>
-    <t>A GATT characteristic in the remote GATT database was discovered</t>
-  </si>
-  <si>
     <t>sl_bt_evt_gatt_characteristic_value_id</t>
   </si>
   <si>
@@ -119,12 +113,6 @@
   </si>
   <si>
     <t>Things to be aware of: _x000D_Scanning is now controlled by a software component. The Bluetooth SoC Empty project includes software component "Scanner for legacy advertisements” which creates event sl_bt_evt_scanner_legacy_advertisement_report_id, which is what we are currently doing in our Sever implementations (sending what SiLabs refers to as legacy advertisements).</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <r>
@@ -164,13 +152,7 @@
     <t>Start scanning for server again (for new potential connection)</t>
   </si>
   <si>
-    <t>Look for Temperature Measurement Characteristic (uuid = 0x2A1C)</t>
-  </si>
-  <si>
     <t>sl_bt_gatt_set_characteristic_notification()</t>
-  </si>
-  <si>
-    <t>Set indication for Temp. Measurement (uuid = 0x2A1C)</t>
   </si>
   <si>
     <r>
@@ -223,46 +205,113 @@
     </r>
   </si>
   <si>
+    <t>Discovered Temperature Measurement Characteristic (uuid = 0x2A1C), store data for state update later</t>
+  </si>
+  <si>
+    <t>Discovered Health Thermometer Service(uuid = 0x1809), store data for state update later</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_scanner_legacy_advertisement_report_id</t>
+  </si>
+  <si>
+    <t>sl_bt_system_get_identity_address()</t>
+  </si>
+  <si>
+    <t>To get address of device</t>
+  </si>
+  <si>
+    <t>only when STATE = CLIENT_CHECK_GATT_SERVICE
+Look for Temperature Measurement Characteristic (uuid = 0x2A1C)</t>
+  </si>
+  <si>
+    <t>only when STATE = CLIENT_CHECK_GATT_CHARACTERSTIC
+Set indication for Temp. Measurement (uuid = 0x2A1C)</t>
+  </si>
+  <si>
+    <t>only when CLIENT_SET_GATT_INDICATION
+no ble function called, update flag for indication</t>
+  </si>
+  <si>
+    <t>update_flag_for_indication()</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>If temperature measurement value</t>
+      <t xml:space="preserve">A GATT service in the remote GATT database was discovered
+</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="8"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">,  displayPrintf() - non BLE function, to display temperature </t>
+      <t>update_flag_for_service()</t>
     </r>
   </si>
   <si>
-    <t>Discovered Temperature Measurement Characteristic (uuid = 0x2A1C), store data for state update later</t>
-  </si>
-  <si>
-    <t>Indication enabled for Temperature Measurement (uuid = 0x2A1C), store data for state update later</t>
-  </si>
-  <si>
-    <t>Discovered Health Thermometer Service(uuid = 0x1809), store data for state update later</t>
-  </si>
-  <si>
-    <t>Only for temperature indication</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_scanner_legacy_advertisement_report_id</t>
+    <r>
+      <t xml:space="preserve">A GATT characteristic in the remote GATT database was discovered
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>update_flag_for_characteristic()</t>
+    </r>
+  </si>
+  <si>
+    <t>Indication enabled for Temperature Measurement (uuid = 0x2A1C)</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_NAME, "Client"
+DISPLAY_ROW_BTADDR, client_addr
+DISPLAY_ROW_CONNECTION, "Discovering"
+DISPLAY_ROW_ASSIGNMENT, "A7"</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_CONNECTION, "Connected"
+DISPLAY_ROW_BTADDR2, server_addr</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_CONNECTION, "Discovering"
+DISPLAY_ROW_BTADDR2, ""
+DISPLAY_ROW_TEMPVALUE, ""</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_CONNECTION, "Handling Indications"</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_TEMPVALUE, "Temp=%d", temperature</t>
+  </si>
+  <si>
+    <t>X (BLE_OFF -&gt; SCANNING)</t>
+  </si>
+  <si>
+    <t>X (SCANNING -&gt; GATT_SERVICE)</t>
+  </si>
+  <si>
+    <t>X (GATT_CHARACTERISTIC -&gt; GATT_INDICATION</t>
+  </si>
+  <si>
+    <t>X (GATT_INDICATION -&gt; RECEIVE_TEMP_DATA)</t>
+  </si>
+  <si>
+    <t>X (GATT_SERVICE -&gt; GATT_CHARACTERISTIC)</t>
+  </si>
+  <si>
+    <t>X (ANY_STATE -&gt; SCANNING)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -296,11 +345,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="14"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FFE46C0A"/>
       <name val="Calibri"/>
     </font>
@@ -330,12 +374,6 @@
     <font>
       <sz val="10"/>
       <color indexed="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -463,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -506,10 +544,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -517,19 +552,40 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -632,22 +688,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>821121</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>32844</xdr:rowOff>
+      <xdr:colOff>798383</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>125422</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1520935</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>115353</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>16033</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>121533</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{406AF408-2E0B-60C7-7199-ED406DA2ADDE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6002149-4F9C-8E06-2C05-AF8A5BA4422B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -669,8 +725,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="821121" y="10959223"/>
-          <a:ext cx="7772400" cy="5162509"/>
+          <a:off x="798383" y="12342270"/>
+          <a:ext cx="7773585" cy="5388089"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1760,18 +1816,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="87" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19" style="1" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28" style="1" customWidth="1"/>
     <col min="5" max="5" width="49.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="74" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" style="1" customWidth="1"/>
@@ -1780,13 +1836,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1807,8 +1863,8 @@
       <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>35</v>
+      <c r="E3" s="23" t="s">
+        <v>31</v>
       </c>
       <c r="F3" s="5"/>
     </row>
@@ -1845,280 +1901,304 @@
       <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E8" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E9" s="37"/>
+      <c r="F9" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="37"/>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="13" t="s">
-        <v>34</v>
-      </c>
+      <c r="D11" s="13"/>
       <c r="E11" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="C12" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="17" t="s">
-        <v>19</v>
-      </c>
+      <c r="B13" s="4"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
     </row>
-    <row r="14" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23" t="s">
+    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="16" t="s">
+      <c r="C17" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F17" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
-      <c r="B18" s="17" t="s">
-        <v>21</v>
-      </c>
+      <c r="B18" s="4"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
-      <c r="E18" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="B19" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
+      <c r="E19" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
     </row>
-    <row r="21" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="17" t="s">
-        <v>52</v>
-      </c>
+    <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="4"/>
       <c r="C21" s="16"/>
-      <c r="D21" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>44</v>
-      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
       <c r="F21" s="16"/>
     </row>
-    <row r="22" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E23" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>40</v>
+      <c r="D24" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
+      <c r="D25" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="E25" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" s="16"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="18" t="s">
-        <v>29</v>
+      <c r="D27" s="25"/>
+      <c r="E27" s="24" t="s">
+        <v>50</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="25" t="s">
-        <v>43</v>
+      <c r="D28" s="25"/>
+      <c r="E28" s="24" t="s">
+        <v>51</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E8:E10"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>